<commit_message>
menambahkan link google fonts dan font awesome
</commit_message>
<xml_diff>
--- a/pengenalan web dasar/Cheklist Submission.xlsx
+++ b/pengenalan web dasar/Cheklist Submission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dicodingtutorial\pengenalan web dasar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284E1FAE-1332-4DBD-9B86-ED4B9CF81ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665B1393-56E9-4E24-AAF1-0D8D4C8A0994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{ACFF2887-0C1F-4C33-87A1-DFA6EC3E257F}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{ACFF2887-0C1F-4C33-87A1-DFA6EC3E257F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Terdapat</t>
   </si>
@@ -194,6 +194,9 @@
   </si>
   <si>
     <t>Menggunakan library Bootstrap, Materialize, Foundation, untuk menyusun layout</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -239,12 +242,12 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -630,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE0CF76-BDD3-4012-8AF9-D047F3609AA5}">
   <dimension ref="B2:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="52" workbookViewId="0">
-      <selection activeCell="X31" sqref="X31"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,7 +648,7 @@
       <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="4"/>
       <c r="O2" s="5" t="s">
         <v>18</v>
       </c>
@@ -655,16 +658,19 @@
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
       <c r="C4" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -704,7 +710,7 @@
       <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="4" t="s">
+      <c r="O10" s="1" t="s">
         <v>25</v>
       </c>
     </row>
@@ -733,7 +739,7 @@
       <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -774,7 +780,7 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="O22" s="4" t="s">
+      <c r="O22" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -802,7 +808,7 @@
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ceklis berapa kriteria dari submission
</commit_message>
<xml_diff>
--- a/pengenalan web dasar/Cheklist Submission.xlsx
+++ b/pengenalan web dasar/Cheklist Submission.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dicodingtutorial\pengenalan web dasar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665B1393-56E9-4E24-AAF1-0D8D4C8A0994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E315E5-9D92-4E36-A4E9-528965D7D339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{ACFF2887-0C1F-4C33-87A1-DFA6EC3E257F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ACFF2887-0C1F-4C33-87A1-DFA6EC3E257F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>Terdapat</t>
   </si>
@@ -197,6 +197,18 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>Fitur tambahan</t>
+  </si>
+  <si>
+    <t>tambahkan kolom komentar</t>
+  </si>
+  <si>
+    <t>tambahkan tentang website ini</t>
+  </si>
+  <si>
+    <t>tambahkan list artikel</t>
   </si>
 </sst>
 </file>
@@ -631,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE0CF76-BDD3-4012-8AF9-D047F3609AA5}">
-  <dimension ref="B2:R33"/>
+  <dimension ref="B2:AI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,9 +654,10 @@
     <col min="2" max="2" width="3.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.140625" customWidth="1"/>
     <col min="15" max="15" width="4.28515625" customWidth="1"/>
+    <col min="34" max="34" width="4.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
@@ -656,14 +669,20 @@
       <c r="R2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="AH2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="AI3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>42</v>
       </c>
@@ -673,16 +692,28 @@
       <c r="O4" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="AI4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
       <c r="C5" t="s">
         <v>2</v>
       </c>
       <c r="P5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="AI5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -690,7 +721,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -698,7 +732,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
@@ -706,7 +743,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:35" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -714,7 +751,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
@@ -722,7 +762,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
@@ -730,12 +773,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
       <c r="C13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
       <c r="C14" t="s">
         <v>10</v>
       </c>
@@ -743,12 +792,15 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:35" x14ac:dyDescent="0.25">
       <c r="P15" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:35" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
       <c r="C16" t="s">
         <v>11</v>
       </c>
@@ -770,11 +822,17 @@
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
       <c r="C19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
       <c r="C21" t="s">
         <v>14</v>
       </c>
@@ -785,6 +843,9 @@
       </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
       <c r="C23" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
mengubah nama folder project
</commit_message>
<xml_diff>
--- a/pengenalan web dasar/Cheklist Submission.xlsx
+++ b/pengenalan web dasar/Cheklist Submission.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\dicodingtutorial\pengenalan web dasar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E315E5-9D92-4E36-A4E9-528965D7D339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD852C8-3A3F-49F5-87FD-77846E533D10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{ACFF2887-0C1F-4C33-87A1-DFA6EC3E257F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Terdapat</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>tambahkan list artikel</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -645,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE0CF76-BDD3-4012-8AF9-D047F3609AA5}">
   <dimension ref="B2:AI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="AI6" sqref="AI6"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,6 +761,9 @@
       <c r="C11" t="s">
         <v>7</v>
       </c>
+      <c r="O11" t="s">
+        <v>47</v>
+      </c>
       <c r="P11" t="s">
         <v>26</v>
       </c>
@@ -768,6 +774,9 @@
       </c>
       <c r="C12" t="s">
         <v>8</v>
+      </c>
+      <c r="O12" t="s">
+        <v>47</v>
       </c>
       <c r="P12" t="s">
         <v>27</v>

</xml_diff>